<commit_message>
Fixed up not_imputed elections
</commit_message>
<xml_diff>
--- a/data/elections/not_imputed/Congressional Elections (2000).xlsx
+++ b/data/elections/not_imputed/Congressional Elections (2000).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/data/elections/not_imputed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFC129B-AD2E-BE49-A7E7-38939F2C368A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5BABDA-8BBD-344E-AED8-AA232C01A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="500" windowWidth="23020" windowHeight="15560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="9920" windowWidth="23020" windowHeight="15560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Election Results by State" sheetId="2" r:id="rId1"/>
@@ -380,7 +380,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -405,14 +405,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -457,16 +449,16 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,57 +742,57 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C49" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A51"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="7"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="12.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="8"/>
+    <col min="5" max="6" width="10.83203125" style="9"/>
+    <col min="7" max="7" width="12.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -814,20 +806,20 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="8">
         <v>849229</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="9">
         <v>485660</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="10">
         <f t="shared" ref="F2:F51" si="0">G2-E2-D2</f>
         <v>104105</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="9">
         <v>1438994</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="4">
         <f t="shared" ref="H2:H33" si="1">K2-I2-J2</f>
         <v>5</v>
       </c>
@@ -851,20 +843,20 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="8">
         <v>190862</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="9">
         <v>45372</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="10">
         <f t="shared" si="0"/>
         <v>38159</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="9">
         <v>274393</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -888,20 +880,20 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="8">
         <v>854715</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="9">
         <v>557849</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="10">
         <f t="shared" si="0"/>
         <v>53092</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="9">
         <v>1465656</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -925,20 +917,20 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="8">
         <v>277146</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="9">
         <v>355366</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="10">
         <f t="shared" si="0"/>
         <v>253</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="9">
         <v>632765</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -962,20 +954,20 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="8">
         <v>4446295</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="9">
         <v>5406623</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="10">
         <f t="shared" si="0"/>
         <v>583689</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="9">
         <v>10436607</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="4">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
@@ -999,20 +991,20 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>968651</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="9">
         <v>496045</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="10">
         <f t="shared" si="0"/>
         <v>159186</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="9">
         <v>1623882</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1036,20 +1028,20 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="8">
         <v>590689</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="9">
         <v>699237</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="10">
         <f t="shared" si="0"/>
         <v>23564</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="9">
         <v>1313490</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1073,20 +1065,20 @@
       <c r="C9" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="8">
         <v>211797</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="9">
         <v>96488</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="10">
         <f t="shared" si="0"/>
         <v>4841</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="9">
         <v>313126</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1110,20 +1102,20 @@
       <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="8">
         <v>2851623</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="9">
         <v>1976189</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="10">
         <f t="shared" si="0"/>
         <v>183408</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="9">
         <v>5011220</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="4">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
@@ -1147,20 +1139,20 @@
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="8">
         <v>1498337</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="9">
         <v>918085</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="10">
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="9">
         <v>2416622</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="4">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -1184,20 +1176,20 @@
       <c r="C12" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="8">
         <v>110895</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="9">
         <v>221373</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="10">
         <f t="shared" si="0"/>
         <v>8156</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="9">
         <v>340424</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1221,20 +1213,20 @@
       <c r="C13" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="8">
         <v>332655</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="9">
         <v>142345</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="10">
         <f t="shared" si="0"/>
         <v>17835</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="9">
         <v>492835</v>
       </c>
-      <c r="H13" s="9">
+      <c r="H13" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1258,20 +1250,20 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="8">
         <v>1907306</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="9">
         <v>2453674</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="10">
         <f t="shared" si="0"/>
         <v>32306</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="9">
         <v>4393286</v>
       </c>
-      <c r="H14" s="9">
+      <c r="H14" s="4">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -1295,20 +1287,20 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="8">
         <v>1140554</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="9">
         <v>953167</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="10">
         <f t="shared" si="0"/>
         <v>63023</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="9">
         <v>2156744</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1332,20 +1324,20 @@
       <c r="C16" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="8">
         <v>717322</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="9">
         <v>531642</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="10">
         <f t="shared" si="0"/>
         <v>26970</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="9">
         <v>1275934</v>
       </c>
-      <c r="H16" s="9">
+      <c r="H16" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1369,20 +1361,20 @@
       <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="8">
         <v>655822</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="9">
         <v>328194</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="10">
         <f t="shared" si="0"/>
         <v>51945</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="9">
         <v>1035961</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1406,20 +1398,20 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="8">
         <v>824915</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="9">
         <v>561752</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="10">
         <f t="shared" si="0"/>
         <v>48742</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="9">
         <v>1435409</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1443,20 +1435,20 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="8">
         <v>747115</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="9">
         <v>359668</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="10">
         <f t="shared" si="0"/>
         <v>95388</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="9">
         <v>1202171</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1480,20 +1472,20 @@
       <c r="C20" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="8">
         <v>203437</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="9">
         <v>422606</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="10">
         <f t="shared" si="0"/>
         <v>12356</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="9">
         <v>638399</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1517,20 +1509,20 @@
       <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="8">
         <v>856306</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="9">
         <v>1060934</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="10">
         <f t="shared" si="0"/>
         <v>9524</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="9">
         <v>1926764</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="4">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -1554,20 +1546,20 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="8">
         <v>343498</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="9">
         <v>1967942</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="10">
         <f t="shared" si="0"/>
         <v>422532</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="9">
         <v>2733972</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1591,20 +1583,20 @@
       <c r="C23" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="8">
         <v>1786980</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="9">
         <v>2177618</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="10">
         <f t="shared" si="0"/>
         <v>105062</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="9">
         <v>4069660</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="4">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -1628,20 +1620,20 @@
       <c r="C24" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="8">
         <v>993371</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="9">
         <v>1234204</v>
       </c>
-      <c r="F24" s="8">
+      <c r="F24" s="10">
         <f t="shared" si="0"/>
         <v>136163</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="9">
         <v>2363738</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1665,20 +1657,20 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="8">
         <v>468483</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="9">
         <v>495687</v>
       </c>
-      <c r="F25" s="8">
+      <c r="F25" s="10">
         <f t="shared" si="0"/>
         <v>21969</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="9">
         <v>986139</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1702,20 +1694,20 @@
       <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="8">
         <v>1135724</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="9">
         <v>1136020</v>
       </c>
-      <c r="F26" s="8">
+      <c r="F26" s="10">
         <f t="shared" si="0"/>
         <v>54044</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="9">
         <v>2325788</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="4">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1739,20 +1731,20 @@
       <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="8">
         <v>211418</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="9">
         <v>189971</v>
       </c>
-      <c r="F27" s="8">
+      <c r="F27" s="10">
         <f t="shared" si="0"/>
         <v>9132</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="9">
         <v>410521</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1776,20 +1768,20 @@
       <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="8">
         <v>486513</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="9">
         <v>178071</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="10">
         <f t="shared" si="0"/>
         <v>18487</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="9">
         <v>683071</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1813,20 +1805,20 @@
       <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="8">
         <v>330884</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="9">
         <v>224848</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="10">
         <f t="shared" si="0"/>
         <v>30921</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G29" s="9">
         <v>586653</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1850,20 +1842,20 @@
       <c r="C30" t="s">
         <v>57</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="8">
         <v>303190</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="9">
         <v>238754</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F30" s="10">
         <f t="shared" si="0"/>
         <v>14105</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="9">
         <v>556049</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1887,20 +1879,20 @@
       <c r="C31" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="8">
         <v>1384170</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="9">
         <v>1532240</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F31" s="10">
         <f t="shared" si="0"/>
         <v>71823</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="9">
         <v>2988233</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="4">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -1924,20 +1916,20 @@
       <c r="C32" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="8">
         <v>274017</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="9">
         <v>299841</v>
       </c>
-      <c r="F32" s="8">
+      <c r="F32" s="10">
         <f t="shared" si="0"/>
         <v>13656</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="9">
         <v>587514</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1961,20 +1953,20 @@
       <c r="C33" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="8">
         <v>2235461</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="9">
         <v>3051701</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="10">
         <f t="shared" si="0"/>
         <v>1661514</v>
       </c>
-      <c r="G33" s="1">
+      <c r="G33" s="9">
         <v>6948676</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="4">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -1998,20 +1990,20 @@
       <c r="C34" t="s">
         <v>65</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="8">
         <v>1514806</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="9">
         <v>1193600</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="10">
         <f t="shared" si="0"/>
         <v>71394</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="9">
         <v>2779800</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="4">
         <f t="shared" ref="H34:H50" si="2">K34-I34-J34</f>
         <v>7</v>
       </c>
@@ -2035,20 +2027,20 @@
       <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="8">
         <v>127251</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="9">
         <v>151173</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="10">
         <f t="shared" si="0"/>
         <v>7234</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="9">
         <v>285658</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2072,20 +2064,20 @@
       <c r="C36" t="s">
         <v>69</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="8">
         <v>2235463</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="9">
         <v>2098854</v>
       </c>
-      <c r="F36" s="8">
+      <c r="F36" s="10">
         <f t="shared" si="0"/>
         <v>250721</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="9">
         <v>4585038</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="4">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -2109,20 +2101,20 @@
       <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="8">
         <v>701820</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="9">
         <v>336955</v>
       </c>
-      <c r="F37" s="8">
+      <c r="F37" s="10">
         <f t="shared" si="0"/>
         <v>48740</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="9">
         <v>1087515</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -2146,20 +2138,20 @@
       <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="8">
         <v>607098</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="9">
         <v>790365</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="10">
         <f t="shared" si="0"/>
         <v>42539</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="9">
         <v>1440002</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2183,20 +2175,20 @@
       <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="8">
         <v>2229057</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="9">
         <v>2279227</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="10">
         <f t="shared" si="0"/>
         <v>43726</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="9">
         <v>4552010</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="4">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
@@ -2220,20 +2212,20 @@
       <c r="C40" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="8">
         <v>89454</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="9">
         <v>247247</v>
       </c>
-      <c r="F40" s="8">
+      <c r="F40" s="10">
         <f t="shared" si="0"/>
         <v>47571</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="9">
         <v>384272</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2257,20 +2249,20 @@
       <c r="C41" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="8">
         <v>729803</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="9">
         <v>523141</v>
       </c>
-      <c r="F41" s="8">
+      <c r="F41" s="10">
         <f t="shared" si="0"/>
         <v>68368</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="9">
         <v>1321312</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -2294,20 +2286,20 @@
       <c r="C42" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="8">
         <v>231083</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="9">
         <v>78321</v>
       </c>
-      <c r="F42" s="8">
+      <c r="F42" s="10">
         <f t="shared" si="0"/>
         <v>5357</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="9">
         <v>314761</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2331,20 +2323,20 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D43" s="8">
         <v>991984</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="9">
         <v>819100</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="10">
         <f t="shared" si="0"/>
         <v>43294</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="9">
         <v>1854378</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="4">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -2368,20 +2360,20 @@
       <c r="C44" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D44" s="8">
         <v>2932411</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="9">
         <v>2799051</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="10">
         <f t="shared" si="0"/>
         <v>254301</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="9">
         <v>5985763</v>
       </c>
-      <c r="H44" s="9">
+      <c r="H44" s="4">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
@@ -2405,20 +2397,20 @@
       <c r="C45" t="s">
         <v>87</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D45" s="8">
         <v>426648</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="9">
         <v>304797</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="10">
         <f t="shared" si="0"/>
         <v>27309</v>
       </c>
-      <c r="G45" s="1">
+      <c r="G45" s="9">
         <v>758754</v>
       </c>
-      <c r="H45" s="9">
+      <c r="H45" s="4">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -2442,20 +2434,20 @@
       <c r="C46" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D46" s="8">
         <v>51977</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="9">
         <v>14918</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="10">
         <f t="shared" si="0"/>
         <v>216471</v>
       </c>
-      <c r="G46" s="1">
+      <c r="G46" s="9">
         <v>283366</v>
       </c>
-      <c r="H46" s="9">
+      <c r="H46" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2479,20 +2471,20 @@
       <c r="C47" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="8">
         <v>1131999</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="9">
         <v>1060484</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="10">
         <f t="shared" si="0"/>
         <v>229246</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="9">
         <v>2421729</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="4">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -2516,20 +2508,20 @@
       <c r="C48" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="8">
         <v>997877</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="9">
         <v>1245872</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="10">
         <f t="shared" si="0"/>
         <v>138662</v>
       </c>
-      <c r="G48" s="1">
+      <c r="G48" s="9">
         <v>2382411</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H48" s="4">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -2553,20 +2545,20 @@
       <c r="C49" t="s">
         <v>95</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="8">
         <v>108769</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="9">
         <v>420784</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="10">
         <f t="shared" si="0"/>
         <v>50319</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="9">
         <v>579872</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="4">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -2590,20 +2582,20 @@
       <c r="C50" t="s">
         <v>97</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="8">
         <v>1311447</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="9">
         <v>1187866</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="10">
         <f t="shared" si="0"/>
         <v>7001</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="9">
         <v>2506314</v>
       </c>
-      <c r="H50" s="9">
+      <c r="H50" s="4">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -2627,20 +2619,20 @@
       <c r="C51" t="s">
         <v>99</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="8">
         <v>141848</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="9">
         <v>60638</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="10">
         <f t="shared" si="0"/>
         <v>9826</v>
       </c>
-      <c r="G51" s="1">
+      <c r="G51" s="9">
         <v>212312</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H51" s="4">
         <f t="shared" ref="H51" si="3">K51-I51-J51</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated not imputed data & vs. imputed comparison
</commit_message>
<xml_diff>
--- a/data/elections/not_imputed/Congressional Elections (2000).xlsx
+++ b/data/elections/not_imputed/Congressional Elections (2000).xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10104"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/dev/MM2/data/elections/not_imputed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5BABDA-8BBD-344E-AED8-AA232C01A6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED95D17-19C8-494F-98EB-5B44389E5AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="9920" windowWidth="23020" windowHeight="15560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2380" yWindow="2440" windowWidth="23020" windowHeight="15560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Election Results by State" sheetId="2" r:id="rId1"/>
+    <sheet name="UPDATED" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Election Results by State'!$K$1:$K$51</definedName>
+    <definedName name="Congressional_Elections__2000" localSheetId="1">UPDATED!$A$1:$J$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,8 +42,29 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{A3F5F6B2-1C99-1743-B33B-6E3844456D69}" name="Congressional Elections (2000)" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="65001" sourceFile="/Users/alecramsay/Documents/dev/MM2/data/elections/not_imputed/Congressional Elections (2000).csv" comma="1">
+      <textFields count="10">
+        <textField type="text"/>
+        <textField type="text"/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="113">
   <si>
     <t>Alabama</t>
   </si>
@@ -374,6 +397,12 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Vote share</t>
   </si>
 </sst>
 </file>
@@ -382,14 +411,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -407,6 +428,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,24 +472,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -474,6 +506,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Congressional Elections (2000)" connectionId="1" xr16:uid="{84AF9C80-B5DB-F145-80FD-CFE5000FD05D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,13 +775,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,7 +789,8 @@
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="8"/>
-    <col min="5" max="6" width="10.83203125" style="9"/>
+    <col min="5" max="5" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="10.83203125" style="12"/>
     <col min="7" max="7" width="12.1640625" style="9" customWidth="1"/>
     <col min="8" max="8" width="6.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
@@ -812,15 +849,13 @@
       <c r="E2" s="9">
         <v>485660</v>
       </c>
-      <c r="F2" s="10">
-        <f t="shared" ref="F2:F51" si="0">G2-E2-D2</f>
+      <c r="F2" s="12">
         <v>104105</v>
       </c>
       <c r="G2" s="9">
         <v>1438994</v>
       </c>
       <c r="H2" s="4">
-        <f t="shared" ref="H2:H33" si="1">K2-I2-J2</f>
         <v>5</v>
       </c>
       <c r="I2">
@@ -849,15 +884,13 @@
       <c r="E3" s="9">
         <v>45372</v>
       </c>
-      <c r="F3" s="10">
-        <f t="shared" si="0"/>
+      <c r="F3" s="12">
         <v>38159</v>
       </c>
       <c r="G3" s="9">
         <v>274393</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I3">
@@ -886,15 +919,13 @@
       <c r="E4" s="9">
         <v>557849</v>
       </c>
-      <c r="F4" s="10">
-        <f t="shared" si="0"/>
+      <c r="F4" s="12">
         <v>53092</v>
       </c>
       <c r="G4" s="9">
         <v>1465656</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I4">
@@ -923,15 +954,13 @@
       <c r="E5" s="9">
         <v>355366</v>
       </c>
-      <c r="F5" s="10">
-        <f t="shared" si="0"/>
+      <c r="F5" s="12">
         <v>253</v>
       </c>
       <c r="G5" s="9">
         <v>632765</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I5">
@@ -960,15 +989,13 @@
       <c r="E6" s="9">
         <v>5406623</v>
       </c>
-      <c r="F6" s="10">
-        <f t="shared" si="0"/>
+      <c r="F6" s="12">
         <v>583689</v>
       </c>
       <c r="G6" s="9">
         <v>10436607</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="I6">
@@ -997,15 +1024,13 @@
       <c r="E7" s="9">
         <v>496045</v>
       </c>
-      <c r="F7" s="10">
-        <f t="shared" si="0"/>
+      <c r="F7" s="12">
         <v>159186</v>
       </c>
       <c r="G7" s="9">
         <v>1623882</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I7">
@@ -1034,15 +1059,13 @@
       <c r="E8" s="9">
         <v>699237</v>
       </c>
-      <c r="F8" s="10">
-        <f t="shared" si="0"/>
+      <c r="F8" s="12">
         <v>23564</v>
       </c>
       <c r="G8" s="9">
         <v>1313490</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I8">
@@ -1071,15 +1094,13 @@
       <c r="E9" s="9">
         <v>96488</v>
       </c>
-      <c r="F9" s="10">
-        <f t="shared" si="0"/>
+      <c r="F9" s="12">
         <v>4841</v>
       </c>
       <c r="G9" s="9">
         <v>313126</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I9">
@@ -1108,15 +1129,13 @@
       <c r="E10" s="9">
         <v>1976189</v>
       </c>
-      <c r="F10" s="10">
-        <f t="shared" si="0"/>
+      <c r="F10" s="12">
         <v>183408</v>
       </c>
       <c r="G10" s="9">
         <v>5011220</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="I10">
@@ -1145,15 +1164,13 @@
       <c r="E11" s="9">
         <v>918085</v>
       </c>
-      <c r="F11" s="10">
-        <f t="shared" si="0"/>
+      <c r="F11" s="12">
         <v>200</v>
       </c>
       <c r="G11" s="9">
         <v>2416622</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="I11">
@@ -1182,15 +1199,13 @@
       <c r="E12" s="9">
         <v>221373</v>
       </c>
-      <c r="F12" s="10">
-        <f t="shared" si="0"/>
+      <c r="F12" s="12">
         <v>8156</v>
       </c>
       <c r="G12" s="9">
         <v>340424</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I12">
@@ -1219,15 +1234,13 @@
       <c r="E13" s="9">
         <v>142345</v>
       </c>
-      <c r="F13" s="10">
-        <f t="shared" si="0"/>
+      <c r="F13" s="12">
         <v>17835</v>
       </c>
       <c r="G13" s="9">
         <v>492835</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I13">
@@ -1256,15 +1269,13 @@
       <c r="E14" s="9">
         <v>2453674</v>
       </c>
-      <c r="F14" s="10">
-        <f t="shared" si="0"/>
+      <c r="F14" s="12">
         <v>32306</v>
       </c>
       <c r="G14" s="9">
         <v>4393286</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="I14">
@@ -1293,15 +1304,13 @@
       <c r="E15" s="9">
         <v>953167</v>
       </c>
-      <c r="F15" s="10">
-        <f t="shared" si="0"/>
+      <c r="F15" s="12">
         <v>63023</v>
       </c>
       <c r="G15" s="9">
         <v>2156744</v>
       </c>
       <c r="H15" s="4">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I15">
@@ -1330,15 +1339,13 @@
       <c r="E16" s="9">
         <v>531642</v>
       </c>
-      <c r="F16" s="10">
-        <f t="shared" si="0"/>
+      <c r="F16" s="12">
         <v>26970</v>
       </c>
       <c r="G16" s="9">
         <v>1275934</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I16">
@@ -1367,15 +1374,13 @@
       <c r="E17" s="9">
         <v>328194</v>
       </c>
-      <c r="F17" s="10">
-        <f t="shared" si="0"/>
+      <c r="F17" s="12">
         <v>51945</v>
       </c>
       <c r="G17" s="9">
         <v>1035961</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I17">
@@ -1404,15 +1409,13 @@
       <c r="E18" s="9">
         <v>561752</v>
       </c>
-      <c r="F18" s="10">
-        <f t="shared" si="0"/>
+      <c r="F18" s="12">
         <v>48742</v>
       </c>
       <c r="G18" s="9">
         <v>1435409</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I18">
@@ -1441,15 +1444,13 @@
       <c r="E19" s="9">
         <v>359668</v>
       </c>
-      <c r="F19" s="10">
-        <f t="shared" si="0"/>
+      <c r="F19" s="12">
         <v>95388</v>
       </c>
       <c r="G19" s="9">
         <v>1202171</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I19">
@@ -1478,15 +1479,13 @@
       <c r="E20" s="9">
         <v>422606</v>
       </c>
-      <c r="F20" s="10">
-        <f t="shared" si="0"/>
+      <c r="F20" s="12">
         <v>12356</v>
       </c>
       <c r="G20" s="9">
         <v>638399</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I20">
@@ -1515,15 +1514,13 @@
       <c r="E21" s="9">
         <v>1060934</v>
       </c>
-      <c r="F21" s="10">
-        <f t="shared" si="0"/>
+      <c r="F21" s="12">
         <v>9524</v>
       </c>
       <c r="G21" s="9">
         <v>1926764</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I21">
@@ -1552,15 +1549,13 @@
       <c r="E22" s="9">
         <v>1967942</v>
       </c>
-      <c r="F22" s="10">
-        <f t="shared" si="0"/>
+      <c r="F22" s="12">
         <v>422532</v>
       </c>
       <c r="G22" s="9">
         <v>2733972</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I22">
@@ -1589,15 +1584,13 @@
       <c r="E23" s="9">
         <v>2177618</v>
       </c>
-      <c r="F23" s="10">
-        <f t="shared" si="0"/>
+      <c r="F23" s="12">
         <v>105062</v>
       </c>
       <c r="G23" s="9">
         <v>4069660</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="I23">
@@ -1626,15 +1619,13 @@
       <c r="E24" s="9">
         <v>1234204</v>
       </c>
-      <c r="F24" s="10">
-        <f t="shared" si="0"/>
+      <c r="F24" s="12">
         <v>136163</v>
       </c>
       <c r="G24" s="9">
         <v>2363738</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I24">
@@ -1663,15 +1654,13 @@
       <c r="E25" s="9">
         <v>495687</v>
       </c>
-      <c r="F25" s="10">
-        <f t="shared" si="0"/>
+      <c r="F25" s="12">
         <v>21969</v>
       </c>
       <c r="G25" s="9">
         <v>986139</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I25">
@@ -1700,15 +1689,13 @@
       <c r="E26" s="9">
         <v>1136020</v>
       </c>
-      <c r="F26" s="10">
-        <f t="shared" si="0"/>
+      <c r="F26" s="12">
         <v>54044</v>
       </c>
       <c r="G26" s="9">
         <v>2325788</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="I26">
@@ -1737,15 +1724,13 @@
       <c r="E27" s="9">
         <v>189971</v>
       </c>
-      <c r="F27" s="10">
-        <f t="shared" si="0"/>
+      <c r="F27" s="12">
         <v>9132</v>
       </c>
       <c r="G27" s="9">
         <v>410521</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I27">
@@ -1774,15 +1759,13 @@
       <c r="E28" s="9">
         <v>178071</v>
       </c>
-      <c r="F28" s="10">
-        <f t="shared" si="0"/>
+      <c r="F28" s="12">
         <v>18487</v>
       </c>
       <c r="G28" s="9">
         <v>683071</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I28">
@@ -1811,15 +1794,13 @@
       <c r="E29" s="9">
         <v>224848</v>
       </c>
-      <c r="F29" s="10">
-        <f t="shared" si="0"/>
+      <c r="F29" s="12">
         <v>30921</v>
       </c>
       <c r="G29" s="9">
         <v>586653</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I29">
@@ -1848,15 +1829,13 @@
       <c r="E30" s="9">
         <v>238754</v>
       </c>
-      <c r="F30" s="10">
-        <f t="shared" si="0"/>
+      <c r="F30" s="12">
         <v>14105</v>
       </c>
       <c r="G30" s="9">
         <v>556049</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I30">
@@ -1885,15 +1864,13 @@
       <c r="E31" s="9">
         <v>1532240</v>
       </c>
-      <c r="F31" s="10">
-        <f t="shared" si="0"/>
+      <c r="F31" s="12">
         <v>71823</v>
       </c>
       <c r="G31" s="9">
         <v>2988233</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I31">
@@ -1922,15 +1899,13 @@
       <c r="E32" s="9">
         <v>299841</v>
       </c>
-      <c r="F32" s="10">
-        <f t="shared" si="0"/>
+      <c r="F32" s="12">
         <v>13656</v>
       </c>
       <c r="G32" s="9">
         <v>587514</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="I32">
@@ -1959,15 +1934,13 @@
       <c r="E33" s="9">
         <v>3051701</v>
       </c>
-      <c r="F33" s="10">
-        <f t="shared" si="0"/>
+      <c r="F33" s="12">
         <v>1661514</v>
       </c>
       <c r="G33" s="9">
         <v>6948676</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="I33">
@@ -1996,15 +1969,13 @@
       <c r="E34" s="9">
         <v>1193600</v>
       </c>
-      <c r="F34" s="10">
-        <f t="shared" si="0"/>
+      <c r="F34" s="12">
         <v>71394</v>
       </c>
       <c r="G34" s="9">
         <v>2779800</v>
       </c>
       <c r="H34" s="4">
-        <f t="shared" ref="H34:H50" si="2">K34-I34-J34</f>
         <v>7</v>
       </c>
       <c r="I34">
@@ -2033,15 +2004,13 @@
       <c r="E35" s="9">
         <v>151173</v>
       </c>
-      <c r="F35" s="10">
-        <f t="shared" si="0"/>
+      <c r="F35" s="12">
         <v>7234</v>
       </c>
       <c r="G35" s="9">
         <v>285658</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I35">
@@ -2070,15 +2039,13 @@
       <c r="E36" s="9">
         <v>2098854</v>
       </c>
-      <c r="F36" s="10">
-        <f t="shared" si="0"/>
+      <c r="F36" s="12">
         <v>250721</v>
       </c>
       <c r="G36" s="9">
         <v>4585038</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I36">
@@ -2107,15 +2074,13 @@
       <c r="E37" s="9">
         <v>336955</v>
       </c>
-      <c r="F37" s="10">
-        <f t="shared" si="0"/>
+      <c r="F37" s="12">
         <v>48740</v>
       </c>
       <c r="G37" s="9">
         <v>1087515</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I37">
@@ -2144,15 +2109,13 @@
       <c r="E38" s="9">
         <v>790365</v>
       </c>
-      <c r="F38" s="10">
-        <f t="shared" si="0"/>
+      <c r="F38" s="12">
         <v>42539</v>
       </c>
       <c r="G38" s="9">
         <v>1440002</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I38">
@@ -2181,15 +2144,13 @@
       <c r="E39" s="9">
         <v>2279227</v>
       </c>
-      <c r="F39" s="10">
-        <f t="shared" si="0"/>
+      <c r="F39" s="12">
         <v>43726</v>
       </c>
       <c r="G39" s="9">
         <v>4552010</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="I39">
@@ -2218,15 +2179,13 @@
       <c r="E40" s="9">
         <v>247247</v>
       </c>
-      <c r="F40" s="10">
-        <f t="shared" si="0"/>
+      <c r="F40" s="12">
         <v>47571</v>
       </c>
       <c r="G40" s="9">
         <v>384272</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I40">
@@ -2255,15 +2214,13 @@
       <c r="E41" s="9">
         <v>523141</v>
       </c>
-      <c r="F41" s="10">
-        <f t="shared" si="0"/>
+      <c r="F41" s="12">
         <v>68368</v>
       </c>
       <c r="G41" s="9">
         <v>1321312</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I41">
@@ -2292,15 +2249,13 @@
       <c r="E42" s="9">
         <v>78321</v>
       </c>
-      <c r="F42" s="10">
-        <f t="shared" si="0"/>
+      <c r="F42" s="12">
         <v>5357</v>
       </c>
       <c r="G42" s="9">
         <v>314761</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I42">
@@ -2329,15 +2284,13 @@
       <c r="E43" s="9">
         <v>819100</v>
       </c>
-      <c r="F43" s="10">
-        <f t="shared" si="0"/>
+      <c r="F43" s="12">
         <v>43294</v>
       </c>
       <c r="G43" s="9">
         <v>1854378</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I43">
@@ -2366,15 +2319,13 @@
       <c r="E44" s="9">
         <v>2799051</v>
       </c>
-      <c r="F44" s="10">
-        <f t="shared" si="0"/>
+      <c r="F44" s="12">
         <v>254301</v>
       </c>
       <c r="G44" s="9">
         <v>5985763</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="I44">
@@ -2403,15 +2354,13 @@
       <c r="E45" s="9">
         <v>304797</v>
       </c>
-      <c r="F45" s="10">
-        <f t="shared" si="0"/>
+      <c r="F45" s="12">
         <v>27309</v>
       </c>
       <c r="G45" s="9">
         <v>758754</v>
       </c>
       <c r="H45" s="4">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I45">
@@ -2440,15 +2389,13 @@
       <c r="E46" s="9">
         <v>14918</v>
       </c>
-      <c r="F46" s="10">
-        <f t="shared" si="0"/>
+      <c r="F46" s="12">
         <v>216471</v>
       </c>
       <c r="G46" s="9">
         <v>283366</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I46">
@@ -2477,15 +2424,13 @@
       <c r="E47" s="9">
         <v>1060484</v>
       </c>
-      <c r="F47" s="10">
-        <f t="shared" si="0"/>
+      <c r="F47" s="12">
         <v>229246</v>
       </c>
       <c r="G47" s="9">
         <v>2421729</v>
       </c>
       <c r="H47" s="4">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I47">
@@ -2514,15 +2459,13 @@
       <c r="E48" s="9">
         <v>1245872</v>
       </c>
-      <c r="F48" s="10">
-        <f t="shared" si="0"/>
+      <c r="F48" s="12">
         <v>138662</v>
       </c>
       <c r="G48" s="9">
         <v>2382411</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I48">
@@ -2551,15 +2494,13 @@
       <c r="E49" s="9">
         <v>420784</v>
       </c>
-      <c r="F49" s="10">
-        <f t="shared" si="0"/>
+      <c r="F49" s="12">
         <v>50319</v>
       </c>
       <c r="G49" s="9">
         <v>579872</v>
       </c>
       <c r="H49" s="4">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I49">
@@ -2588,15 +2529,13 @@
       <c r="E50" s="9">
         <v>1187866</v>
       </c>
-      <c r="F50" s="10">
-        <f t="shared" si="0"/>
+      <c r="F50" s="12">
         <v>7001</v>
       </c>
       <c r="G50" s="9">
         <v>2506314</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="I50">
@@ -2625,15 +2564,13 @@
       <c r="E51" s="9">
         <v>60638</v>
       </c>
-      <c r="F51" s="10">
-        <f t="shared" si="0"/>
+      <c r="F51" s="12">
         <v>9826</v>
       </c>
       <c r="G51" s="9">
         <v>212312</v>
       </c>
       <c r="H51" s="4">
-        <f t="shared" ref="H51" si="3">K51-I51-J51</f>
         <v>1</v>
       </c>
       <c r="I51">
@@ -2643,6 +2580,1672 @@
         <v>0</v>
       </c>
       <c r="K51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" s="11">
+        <f>SUM(E2:E51)/SUM(D2:E51)</f>
+        <v>0.49818264438916521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0FE8A8-C45B-E647-9B7B-3049B4509F62}">
+  <dimension ref="A1:J51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:J1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>849229</v>
+      </c>
+      <c r="D2">
+        <v>485660</v>
+      </c>
+      <c r="E2">
+        <v>104105</v>
+      </c>
+      <c r="F2">
+        <v>1438994</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>190862</v>
+      </c>
+      <c r="D3">
+        <v>45372</v>
+      </c>
+      <c r="E3">
+        <v>38159</v>
+      </c>
+      <c r="F3">
+        <v>274393</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>854715</v>
+      </c>
+      <c r="D4">
+        <v>557849</v>
+      </c>
+      <c r="E4">
+        <v>53092</v>
+      </c>
+      <c r="F4">
+        <v>1465656</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>277146</v>
+      </c>
+      <c r="D5">
+        <v>355366</v>
+      </c>
+      <c r="E5">
+        <v>253</v>
+      </c>
+      <c r="F5">
+        <v>632765</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>4446295</v>
+      </c>
+      <c r="D6">
+        <v>5406623</v>
+      </c>
+      <c r="E6">
+        <v>583689</v>
+      </c>
+      <c r="F6">
+        <v>10436607</v>
+      </c>
+      <c r="G6">
+        <v>20</v>
+      </c>
+      <c r="H6">
+        <v>32</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>968651</v>
+      </c>
+      <c r="D7">
+        <v>496045</v>
+      </c>
+      <c r="E7">
+        <v>159186</v>
+      </c>
+      <c r="F7">
+        <v>1623882</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>590689</v>
+      </c>
+      <c r="D8">
+        <v>699237</v>
+      </c>
+      <c r="E8">
+        <v>23564</v>
+      </c>
+      <c r="F8">
+        <v>1313490</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>211797</v>
+      </c>
+      <c r="D9">
+        <v>96488</v>
+      </c>
+      <c r="E9">
+        <v>4841</v>
+      </c>
+      <c r="F9">
+        <v>313126</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10">
+        <v>2851623</v>
+      </c>
+      <c r="D10">
+        <v>1976189</v>
+      </c>
+      <c r="E10">
+        <v>183408</v>
+      </c>
+      <c r="F10">
+        <v>5011220</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11">
+        <v>1498337</v>
+      </c>
+      <c r="D11">
+        <v>918085</v>
+      </c>
+      <c r="E11">
+        <v>200</v>
+      </c>
+      <c r="F11">
+        <v>2416622</v>
+      </c>
+      <c r="G11">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12">
+        <v>110895</v>
+      </c>
+      <c r="D12">
+        <v>221373</v>
+      </c>
+      <c r="E12">
+        <v>8156</v>
+      </c>
+      <c r="F12">
+        <v>340424</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>332655</v>
+      </c>
+      <c r="D13">
+        <v>142345</v>
+      </c>
+      <c r="E13">
+        <v>17835</v>
+      </c>
+      <c r="F13">
+        <v>492835</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14">
+        <v>1907306</v>
+      </c>
+      <c r="D14">
+        <v>2453674</v>
+      </c>
+      <c r="E14">
+        <v>32306</v>
+      </c>
+      <c r="F14">
+        <v>4393286</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
+        <v>1140554</v>
+      </c>
+      <c r="D15">
+        <v>953167</v>
+      </c>
+      <c r="E15">
+        <v>63023</v>
+      </c>
+      <c r="F15">
+        <v>2156744</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>717322</v>
+      </c>
+      <c r="D16">
+        <v>531642</v>
+      </c>
+      <c r="E16">
+        <v>26970</v>
+      </c>
+      <c r="F16">
+        <v>1275934</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>655822</v>
+      </c>
+      <c r="D17">
+        <v>328194</v>
+      </c>
+      <c r="E17">
+        <v>51945</v>
+      </c>
+      <c r="F17">
+        <v>1035961</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>824915</v>
+      </c>
+      <c r="D18">
+        <v>561752</v>
+      </c>
+      <c r="E18">
+        <v>48742</v>
+      </c>
+      <c r="F18">
+        <v>1435409</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19">
+        <v>747115</v>
+      </c>
+      <c r="D19">
+        <v>359668</v>
+      </c>
+      <c r="E19">
+        <v>95388</v>
+      </c>
+      <c r="F19">
+        <v>1202171</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>203437</v>
+      </c>
+      <c r="D20">
+        <v>422606</v>
+      </c>
+      <c r="E20">
+        <v>12356</v>
+      </c>
+      <c r="F20">
+        <v>638399</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21">
+        <v>856306</v>
+      </c>
+      <c r="D21">
+        <v>1060934</v>
+      </c>
+      <c r="E21">
+        <v>9524</v>
+      </c>
+      <c r="F21">
+        <v>1926764</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>343498</v>
+      </c>
+      <c r="D22">
+        <v>1967942</v>
+      </c>
+      <c r="E22">
+        <v>422532</v>
+      </c>
+      <c r="F22">
+        <v>2733972</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>10</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23">
+        <v>1786980</v>
+      </c>
+      <c r="D23">
+        <v>2177618</v>
+      </c>
+      <c r="E23">
+        <v>105062</v>
+      </c>
+      <c r="F23">
+        <v>4069660</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24">
+        <v>993371</v>
+      </c>
+      <c r="D24">
+        <v>1234204</v>
+      </c>
+      <c r="E24">
+        <v>136163</v>
+      </c>
+      <c r="F24">
+        <v>2363738</v>
+      </c>
+      <c r="G24">
+        <v>3</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25">
+        <v>468483</v>
+      </c>
+      <c r="D25">
+        <v>495687</v>
+      </c>
+      <c r="E25">
+        <v>21969</v>
+      </c>
+      <c r="F25">
+        <v>986139</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26">
+        <v>1135724</v>
+      </c>
+      <c r="D26">
+        <v>1136020</v>
+      </c>
+      <c r="E26">
+        <v>54044</v>
+      </c>
+      <c r="F26">
+        <v>2325788</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27">
+        <v>211418</v>
+      </c>
+      <c r="D27">
+        <v>189971</v>
+      </c>
+      <c r="E27">
+        <v>9132</v>
+      </c>
+      <c r="F27">
+        <v>410521</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28">
+        <v>486513</v>
+      </c>
+      <c r="D28">
+        <v>178071</v>
+      </c>
+      <c r="E28">
+        <v>18487</v>
+      </c>
+      <c r="F28">
+        <v>683071</v>
+      </c>
+      <c r="G28">
+        <v>3</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29">
+        <v>330884</v>
+      </c>
+      <c r="D29">
+        <v>224848</v>
+      </c>
+      <c r="E29">
+        <v>30921</v>
+      </c>
+      <c r="F29">
+        <v>586653</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30">
+        <v>303190</v>
+      </c>
+      <c r="D30">
+        <v>238754</v>
+      </c>
+      <c r="E30">
+        <v>14105</v>
+      </c>
+      <c r="F30">
+        <v>556049</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31">
+        <v>1384170</v>
+      </c>
+      <c r="D31">
+        <v>1532240</v>
+      </c>
+      <c r="E31">
+        <v>71823</v>
+      </c>
+      <c r="F31">
+        <v>2988233</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32">
+        <v>274017</v>
+      </c>
+      <c r="D32">
+        <v>299841</v>
+      </c>
+      <c r="E32">
+        <v>13656</v>
+      </c>
+      <c r="F32">
+        <v>587514</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33">
+        <v>2235461</v>
+      </c>
+      <c r="D33">
+        <v>3051701</v>
+      </c>
+      <c r="E33">
+        <v>1661514</v>
+      </c>
+      <c r="F33">
+        <v>6948676</v>
+      </c>
+      <c r="G33">
+        <v>12</v>
+      </c>
+      <c r="H33">
+        <v>19</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>1514806</v>
+      </c>
+      <c r="D34">
+        <v>1193600</v>
+      </c>
+      <c r="E34">
+        <v>71394</v>
+      </c>
+      <c r="F34">
+        <v>2779800</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35">
+        <v>127251</v>
+      </c>
+      <c r="D35">
+        <v>151173</v>
+      </c>
+      <c r="E35">
+        <v>7234</v>
+      </c>
+      <c r="F35">
+        <v>285658</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36">
+        <v>2235463</v>
+      </c>
+      <c r="D36">
+        <v>2098854</v>
+      </c>
+      <c r="E36">
+        <v>250721</v>
+      </c>
+      <c r="F36">
+        <v>4585038</v>
+      </c>
+      <c r="G36">
+        <v>11</v>
+      </c>
+      <c r="H36">
+        <v>8</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37">
+        <v>701820</v>
+      </c>
+      <c r="D37">
+        <v>336955</v>
+      </c>
+      <c r="E37">
+        <v>48740</v>
+      </c>
+      <c r="F37">
+        <v>1087515</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38">
+        <v>607098</v>
+      </c>
+      <c r="D38">
+        <v>790365</v>
+      </c>
+      <c r="E38">
+        <v>42539</v>
+      </c>
+      <c r="F38">
+        <v>1440002</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39">
+        <v>2229057</v>
+      </c>
+      <c r="D39">
+        <v>2279227</v>
+      </c>
+      <c r="E39">
+        <v>43726</v>
+      </c>
+      <c r="F39">
+        <v>4552010</v>
+      </c>
+      <c r="G39">
+        <v>11</v>
+      </c>
+      <c r="H39">
+        <v>10</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40">
+        <v>89454</v>
+      </c>
+      <c r="D40">
+        <v>247247</v>
+      </c>
+      <c r="E40">
+        <v>47571</v>
+      </c>
+      <c r="F40">
+        <v>384272</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41">
+        <v>729803</v>
+      </c>
+      <c r="D41">
+        <v>523141</v>
+      </c>
+      <c r="E41">
+        <v>68368</v>
+      </c>
+      <c r="F41">
+        <v>1321312</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42">
+        <v>231083</v>
+      </c>
+      <c r="D42">
+        <v>78321</v>
+      </c>
+      <c r="E42">
+        <v>5357</v>
+      </c>
+      <c r="F42">
+        <v>314761</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43">
+        <v>991984</v>
+      </c>
+      <c r="D43">
+        <v>819100</v>
+      </c>
+      <c r="E43">
+        <v>43294</v>
+      </c>
+      <c r="F43">
+        <v>1854378</v>
+      </c>
+      <c r="G43">
+        <v>5</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44">
+        <v>2932411</v>
+      </c>
+      <c r="D44">
+        <v>2799051</v>
+      </c>
+      <c r="E44">
+        <v>254301</v>
+      </c>
+      <c r="F44">
+        <v>5985763</v>
+      </c>
+      <c r="G44">
+        <v>13</v>
+      </c>
+      <c r="H44">
+        <v>17</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45">
+        <v>426648</v>
+      </c>
+      <c r="D45">
+        <v>304797</v>
+      </c>
+      <c r="E45">
+        <v>27309</v>
+      </c>
+      <c r="F45">
+        <v>758754</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46">
+        <v>51977</v>
+      </c>
+      <c r="D46">
+        <v>14918</v>
+      </c>
+      <c r="E46">
+        <v>216471</v>
+      </c>
+      <c r="F46">
+        <v>283366</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C47">
+        <v>1131999</v>
+      </c>
+      <c r="D47">
+        <v>1060484</v>
+      </c>
+      <c r="E47">
+        <v>229246</v>
+      </c>
+      <c r="F47">
+        <v>2421729</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48">
+        <v>997877</v>
+      </c>
+      <c r="D48">
+        <v>1245872</v>
+      </c>
+      <c r="E48">
+        <v>138662</v>
+      </c>
+      <c r="F48">
+        <v>2382411</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>6</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49">
+        <v>108769</v>
+      </c>
+      <c r="D49">
+        <v>420784</v>
+      </c>
+      <c r="E49">
+        <v>50319</v>
+      </c>
+      <c r="F49">
+        <v>579872</v>
+      </c>
+      <c r="G49">
+        <v>1</v>
+      </c>
+      <c r="H49">
+        <v>2</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50">
+        <v>1311447</v>
+      </c>
+      <c r="D50">
+        <v>1187866</v>
+      </c>
+      <c r="E50">
+        <v>7001</v>
+      </c>
+      <c r="F50">
+        <v>2506314</v>
+      </c>
+      <c r="G50">
+        <v>4</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51">
+        <v>141848</v>
+      </c>
+      <c r="D51">
+        <v>60638</v>
+      </c>
+      <c r="E51">
+        <v>9826</v>
+      </c>
+      <c r="F51">
+        <v>212312</v>
+      </c>
+      <c r="G51">
+        <v>1</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
         <v>1</v>
       </c>
     </row>

</xml_diff>